<commit_message>
added OWID estimate of cases
</commit_message>
<xml_diff>
--- a/debate/cumulative-confirmed-covid-19-cases-deaths-OWID.xlsx
+++ b/debate/cumulative-confirmed-covid-19-cases-deaths-OWID.xlsx
@@ -8,20 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stk\Documents\GitHub\covid\debate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4A9D108A-E464-47DF-A4B6-0DA04FA599D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7ACF13C-7371-4A27-BE6A-3A54FB6C0C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11325" yWindow="2175" windowWidth="14880" windowHeight="11565" xr2:uid="{7A05296F-690E-41E4-A2A9-46AACD6B87B9}"/>
+    <workbookView xWindow="10545" yWindow="2250" windowWidth="25095" windowHeight="11565" xr2:uid="{7A05296F-690E-41E4-A2A9-46AACD6B87B9}"/>
   </bookViews>
   <sheets>
     <sheet name="cumulative-confirmed-covid-19" sheetId="1" r:id="rId1"/>
     <sheet name="Notes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1883" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="21">
   <si>
     <t>Entity</t>
   </si>
@@ -78,6 +91,12 @@
   </si>
   <si>
     <t>definitions</t>
+  </si>
+  <si>
+    <t>found in the covid/debate repo</t>
+  </si>
+  <si>
+    <t>The OWID data above compares favorable to the totals in the wave_regression_cases_deaths_nytimes_data.xls</t>
   </si>
 </sst>
 </file>
@@ -957,7 +976,7 @@
   <dimension ref="A1:I1858"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,11 +1150,11 @@
         <v>10</v>
       </c>
       <c r="G8" s="4">
-        <f>VLOOKUP(G3,$B:$D,2)</f>
+        <f t="shared" ref="G8:H10" si="0">VLOOKUP(G3,$B:$D,2)</f>
         <v>19577585</v>
       </c>
       <c r="H8" s="4">
-        <f>VLOOKUP(H3,$B:$D,2)</f>
+        <f t="shared" si="0"/>
         <v>28330091</v>
       </c>
       <c r="I8" s="4">
@@ -1160,11 +1179,11 @@
         <v>11</v>
       </c>
       <c r="G9" s="4">
-        <f>VLOOKUP(G4,$B:$D,2)</f>
+        <f t="shared" si="0"/>
         <v>33321785</v>
       </c>
       <c r="H9" s="4">
-        <f>VLOOKUP(H4,$B:$D,2)</f>
+        <f t="shared" si="0"/>
         <v>48084683</v>
       </c>
       <c r="I9" s="4">
@@ -1189,11 +1208,11 @@
         <v>12</v>
       </c>
       <c r="G10" s="4">
-        <f>VLOOKUP(G5,$B:$D,2)</f>
+        <f t="shared" si="0"/>
         <v>48178162</v>
       </c>
       <c r="H10" s="4">
-        <f>VLOOKUP(H5,$B:$D,2)</f>
+        <f t="shared" si="0"/>
         <v>79238387</v>
       </c>
       <c r="I10" s="4">
@@ -1287,11 +1306,11 @@
         <v>11</v>
       </c>
       <c r="G14" s="4">
-        <f t="shared" ref="G14:H14" si="0">VLOOKUP(G4,$B:$D,3)</f>
+        <f t="shared" ref="G14:H14" si="1">VLOOKUP(G4,$B:$D,3)</f>
         <v>601201</v>
       </c>
       <c r="H14" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>776038</v>
       </c>
       <c r="I14" s="4">
@@ -1316,11 +1335,11 @@
         <v>12</v>
       </c>
       <c r="G15" s="4">
-        <f t="shared" ref="G15:H15" si="1">VLOOKUP(G5,$B:$D,3)</f>
+        <f t="shared" ref="G15:H15" si="2">VLOOKUP(G5,$B:$D,3)</f>
         <v>777701</v>
       </c>
       <c r="H15" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>972011</v>
       </c>
       <c r="I15" s="4">
@@ -1342,7 +1361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1355,8 +1374,11 @@
       <c r="D17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1369,8 +1391,11 @@
       <c r="D18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1383,8 +1408,17 @@
       <c r="D19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -1397,8 +1431,20 @@
       <c r="D20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="4">
+        <v>8100079</v>
+      </c>
+      <c r="H20" s="4">
+        <v>14380749</v>
+      </c>
+      <c r="I20" s="4">
+        <v>29252506</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -1411,8 +1457,20 @@
       <c r="D21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="4">
+        <v>148033</v>
+      </c>
+      <c r="H21" s="4">
+        <v>160565</v>
+      </c>
+      <c r="I21" s="4">
+        <v>168400</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -1426,7 +1484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -1440,7 +1498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -1454,7 +1512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -1468,7 +1526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -1482,7 +1540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -1496,7 +1554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -1510,7 +1568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -1524,7 +1582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -1538,7 +1596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -1552,7 +1610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>2</v>
       </c>

</xml_diff>